<commit_message>
Payless Readyline and Split Billing Test Scripts and Test Data Sheets
</commit_message>
<xml_diff>
--- a/Payless/TestData/Payless_GUITestData_ReadyLine_Regression.xlsx
+++ b/Payless/TestData/Payless_GUITestData_ReadyLine_Regression.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium\Workspace\ABGAutomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ABG\Payless\TestData\InternetGUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="171">
   <si>
     <t>EXECUTE</t>
   </si>
@@ -513,10 +513,28 @@
     <t>N</t>
   </si>
   <si>
-    <t>https://wizardgui-paylesscar-uat.avisbudget.com/wizardgui/ui/wizard.jsf?mnemonic=</t>
-  </si>
-  <si>
-    <t>Avis0909#</t>
+    <t>https://uat.ccrgservices.com/wizardgui/ui/wizard.jsf?i_brand=i-payless&amp;mnemonic=</t>
+  </si>
+  <si>
+    <t>Avis2018#</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -616,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -677,6 +695,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1235,7 +1262,9 @@
       <c r="BY1" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="BZ1" s="4"/>
+      <c r="BZ1" s="22" t="s">
+        <v>170</v>
+      </c>
       <c r="CA1" s="4"/>
       <c r="CB1" s="4"/>
       <c r="CC1" s="4"/>
@@ -1440,7 +1469,7 @@
       <c r="BW2" s="15"/>
       <c r="BX2" s="15"/>
       <c r="BY2" s="15"/>
-      <c r="BZ2" s="7"/>
+      <c r="BZ2" s="26"/>
       <c r="CA2" s="7"/>
       <c r="CB2" s="7"/>
       <c r="CC2" s="7"/>
@@ -1543,7 +1572,7 @@
       <c r="FV2" s="5"/>
       <c r="FW2" s="5"/>
     </row>
-    <row r="3" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>10</v>
       </c>
@@ -1551,7 +1580,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>83</v>
@@ -1577,8 +1606,8 @@
       <c r="K3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="8">
-        <v>0</v>
+      <c r="L3" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="M3" s="15"/>
       <c r="N3" s="15"/>
@@ -1645,7 +1674,7 @@
       <c r="BW3" s="15"/>
       <c r="BX3" s="15"/>
       <c r="BY3" s="15"/>
-      <c r="BZ3" s="7"/>
+      <c r="BZ3" s="26"/>
       <c r="CA3" s="7"/>
       <c r="CB3" s="7"/>
       <c r="CC3" s="7"/>
@@ -1748,7 +1777,7 @@
       <c r="FV3" s="5"/>
       <c r="FW3" s="5"/>
     </row>
-    <row r="4" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
@@ -1756,7 +1785,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>83</v>
@@ -1782,8 +1811,8 @@
       <c r="K4" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="8">
-        <v>1</v>
+      <c r="L4" s="25" t="s">
+        <v>74</v>
       </c>
       <c r="M4" s="15"/>
       <c r="N4" s="15"/>
@@ -1850,7 +1879,7 @@
       <c r="BW4" s="15"/>
       <c r="BX4" s="15"/>
       <c r="BY4" s="15"/>
-      <c r="BZ4" s="7"/>
+      <c r="BZ4" s="26"/>
       <c r="CA4" s="7"/>
       <c r="CB4" s="7"/>
       <c r="CC4" s="7"/>
@@ -1953,7 +1982,7 @@
       <c r="FV4" s="5"/>
       <c r="FW4" s="5"/>
     </row>
-    <row r="5" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>10</v>
       </c>
@@ -1961,7 +1990,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D5" s="17" t="s">
         <v>83</v>
@@ -1987,8 +2016,8 @@
       <c r="K5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="8">
-        <v>2</v>
+      <c r="L5" s="25" t="s">
+        <v>75</v>
       </c>
       <c r="M5" s="15"/>
       <c r="N5" s="15"/>
@@ -2055,7 +2084,7 @@
       <c r="BW5" s="15"/>
       <c r="BX5" s="15"/>
       <c r="BY5" s="15"/>
-      <c r="BZ5" s="7"/>
+      <c r="BZ5" s="26"/>
       <c r="CA5" s="7"/>
       <c r="CB5" s="7"/>
       <c r="CC5" s="7"/>
@@ -2158,7 +2187,7 @@
       <c r="FV5" s="5"/>
       <c r="FW5" s="5"/>
     </row>
-    <row r="6" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -2166,7 +2195,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>83</v>
@@ -2192,8 +2221,8 @@
       <c r="K6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="8">
-        <v>3</v>
+      <c r="L6" s="25" t="s">
+        <v>165</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
@@ -2260,7 +2289,7 @@
       <c r="BW6" s="15"/>
       <c r="BX6" s="15"/>
       <c r="BY6" s="15"/>
-      <c r="BZ6" s="7"/>
+      <c r="BZ6" s="26"/>
       <c r="CA6" s="7"/>
       <c r="CB6" s="7"/>
       <c r="CC6" s="7"/>
@@ -2363,7 +2392,7 @@
       <c r="FV6" s="5"/>
       <c r="FW6" s="5"/>
     </row>
-    <row r="7" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
@@ -2371,7 +2400,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>83</v>
@@ -2397,8 +2426,8 @@
       <c r="K7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="8">
-        <v>4</v>
+      <c r="L7" s="25" t="s">
+        <v>166</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -2465,7 +2494,7 @@
       <c r="BW7" s="6"/>
       <c r="BX7" s="6"/>
       <c r="BY7" s="6"/>
-      <c r="BZ7" s="7"/>
+      <c r="BZ7" s="26"/>
       <c r="CA7" s="7"/>
       <c r="CB7" s="7"/>
       <c r="CC7" s="7"/>
@@ -2568,7 +2597,7 @@
       <c r="FV7" s="5"/>
       <c r="FW7" s="5"/>
     </row>
-    <row r="8" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>10</v>
       </c>
@@ -2576,7 +2605,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>83</v>
@@ -2670,7 +2699,7 @@
       <c r="BW8" s="6"/>
       <c r="BX8" s="6"/>
       <c r="BY8" s="6"/>
-      <c r="BZ8" s="7"/>
+      <c r="BZ8" s="26"/>
       <c r="CA8" s="7"/>
       <c r="CB8" s="7"/>
       <c r="CC8" s="7"/>
@@ -2773,7 +2802,7 @@
       <c r="FV8" s="5"/>
       <c r="FW8" s="5"/>
     </row>
-    <row r="9" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>10</v>
       </c>
@@ -2781,7 +2810,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>83</v>
@@ -2807,8 +2836,8 @@
       <c r="K9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="8">
-        <v>6</v>
+      <c r="L9" s="25" t="s">
+        <v>167</v>
       </c>
       <c r="M9" s="15"/>
       <c r="N9" s="15"/>
@@ -2875,7 +2904,7 @@
       <c r="BW9" s="6"/>
       <c r="BX9" s="6"/>
       <c r="BY9" s="6"/>
-      <c r="BZ9" s="7"/>
+      <c r="BZ9" s="26"/>
       <c r="CA9" s="7"/>
       <c r="CB9" s="7"/>
       <c r="CC9" s="7"/>
@@ -2978,7 +3007,7 @@
       <c r="FV9" s="5"/>
       <c r="FW9" s="5"/>
     </row>
-    <row r="10" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>10</v>
       </c>
@@ -2986,7 +3015,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>83</v>
@@ -3012,8 +3041,8 @@
       <c r="K10" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L10" s="8">
-        <v>7</v>
+      <c r="L10" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
@@ -3080,7 +3109,7 @@
       <c r="BW10" s="6"/>
       <c r="BX10" s="6"/>
       <c r="BY10" s="6"/>
-      <c r="BZ10" s="7"/>
+      <c r="BZ10" s="26"/>
       <c r="CA10" s="7"/>
       <c r="CB10" s="7"/>
       <c r="CC10" s="7"/>
@@ -3183,7 +3212,7 @@
       <c r="FV10" s="5"/>
       <c r="FW10" s="5"/>
     </row>
-    <row r="11" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>10</v>
       </c>
@@ -3191,7 +3220,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>83</v>
@@ -3217,8 +3246,8 @@
       <c r="K11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="8">
-        <v>8</v>
+      <c r="L11" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
@@ -3285,7 +3314,7 @@
       <c r="BW11" s="6"/>
       <c r="BX11" s="6"/>
       <c r="BY11" s="6"/>
-      <c r="BZ11" s="7"/>
+      <c r="BZ11" s="26"/>
       <c r="CA11" s="7"/>
       <c r="CB11" s="7"/>
       <c r="CC11" s="7"/>
@@ -3388,7 +3417,7 @@
       <c r="FV11" s="5"/>
       <c r="FW11" s="5"/>
     </row>
-    <row r="12" spans="1:179" s="3" customFormat="1" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:179" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -3396,7 +3425,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>83</v>
@@ -3422,8 +3451,8 @@
       <c r="K12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="8">
-        <v>9</v>
+      <c r="L12" s="25" t="s">
+        <v>169</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15"/>
@@ -3490,7 +3519,7 @@
       <c r="BW12" s="6"/>
       <c r="BX12" s="6"/>
       <c r="BY12" s="6"/>
-      <c r="BZ12" s="7"/>
+      <c r="BZ12" s="26"/>
       <c r="CA12" s="7"/>
       <c r="CB12" s="7"/>
       <c r="CC12" s="7"/>
@@ -3695,7 +3724,7 @@
       <c r="BW13" s="6"/>
       <c r="BX13" s="6"/>
       <c r="BY13" s="6"/>
-      <c r="BZ13" s="7"/>
+      <c r="BZ13" s="26"/>
       <c r="CA13" s="7"/>
       <c r="CB13" s="7"/>
       <c r="CC13" s="7"/>
@@ -3900,7 +3929,7 @@
       <c r="BW14" s="6"/>
       <c r="BX14" s="6"/>
       <c r="BY14" s="6"/>
-      <c r="BZ14" s="7"/>
+      <c r="BZ14" s="26"/>
       <c r="CA14" s="7"/>
       <c r="CB14" s="7"/>
       <c r="CC14" s="7"/>
@@ -4105,7 +4134,7 @@
       <c r="BW15" s="6"/>
       <c r="BX15" s="6"/>
       <c r="BY15" s="6"/>
-      <c r="BZ15" s="7"/>
+      <c r="BZ15" s="26"/>
       <c r="CA15" s="7"/>
       <c r="CB15" s="7"/>
       <c r="CC15" s="7"/>
@@ -4704,7 +4733,7 @@
       <c r="FV17" s="5"/>
       <c r="FW17" s="5"/>
     </row>
-    <row r="18" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>10</v>
       </c>
@@ -4712,7 +4741,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>162</v>
+        <v>1</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>83</v>
@@ -4806,7 +4835,7 @@
       <c r="BW18" s="15"/>
       <c r="BX18" s="15"/>
       <c r="BY18" s="15"/>
-      <c r="BZ18" s="10"/>
+      <c r="BZ18" s="27"/>
       <c r="CA18" s="10"/>
       <c r="CB18" s="10"/>
       <c r="CC18" s="10"/>
@@ -4819,7 +4848,7 @@
       <c r="CJ18" s="10"/>
       <c r="CK18" s="10"/>
     </row>
-    <row r="19" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
@@ -4853,8 +4882,8 @@
       <c r="K19" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="L19" s="8">
-        <v>0</v>
+      <c r="L19" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
@@ -4921,7 +4950,7 @@
       <c r="BW19" s="15"/>
       <c r="BX19" s="15"/>
       <c r="BY19" s="15"/>
-      <c r="BZ19" s="10"/>
+      <c r="BZ19" s="27"/>
       <c r="CA19" s="10"/>
       <c r="CB19" s="10"/>
       <c r="CC19" s="10"/>
@@ -4934,7 +4963,7 @@
       <c r="CJ19" s="10"/>
       <c r="CK19" s="10"/>
     </row>
-    <row r="20" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>10</v>
       </c>
@@ -4968,8 +4997,8 @@
       <c r="K20" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="L20" s="8">
-        <v>1</v>
+      <c r="L20" s="25" t="s">
+        <v>74</v>
       </c>
       <c r="M20" s="15"/>
       <c r="N20" s="15"/>
@@ -5036,7 +5065,7 @@
       <c r="BW20" s="15"/>
       <c r="BX20" s="15"/>
       <c r="BY20" s="15"/>
-      <c r="BZ20" s="10"/>
+      <c r="BZ20" s="27"/>
       <c r="CA20" s="10"/>
       <c r="CB20" s="10"/>
       <c r="CC20" s="10"/>
@@ -5049,7 +5078,7 @@
       <c r="CJ20" s="10"/>
       <c r="CK20" s="10"/>
     </row>
-    <row r="21" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>10</v>
       </c>
@@ -5083,8 +5112,8 @@
       <c r="K21" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="L21" s="8">
-        <v>2</v>
+      <c r="L21" s="25" t="s">
+        <v>75</v>
       </c>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
@@ -5151,7 +5180,7 @@
       <c r="BW21" s="15"/>
       <c r="BX21" s="15"/>
       <c r="BY21" s="15"/>
-      <c r="BZ21" s="10"/>
+      <c r="BZ21" s="27"/>
       <c r="CA21" s="10"/>
       <c r="CB21" s="10"/>
       <c r="CC21" s="10"/>
@@ -5164,7 +5193,7 @@
       <c r="CJ21" s="10"/>
       <c r="CK21" s="10"/>
     </row>
-    <row r="22" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>10</v>
       </c>
@@ -5198,8 +5227,8 @@
       <c r="K22" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="8">
-        <v>3</v>
+      <c r="L22" s="25" t="s">
+        <v>165</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -5266,7 +5295,7 @@
       <c r="BW22" s="15"/>
       <c r="BX22" s="15"/>
       <c r="BY22" s="15"/>
-      <c r="BZ22" s="10"/>
+      <c r="BZ22" s="27"/>
       <c r="CA22" s="10"/>
       <c r="CB22" s="10"/>
       <c r="CC22" s="10"/>
@@ -5279,7 +5308,7 @@
       <c r="CJ22" s="10"/>
       <c r="CK22" s="10"/>
     </row>
-    <row r="23" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>10</v>
       </c>
@@ -5313,8 +5342,8 @@
       <c r="K23" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="8">
-        <v>4</v>
+      <c r="L23" s="25" t="s">
+        <v>166</v>
       </c>
       <c r="M23" s="15"/>
       <c r="N23" s="15"/>
@@ -5381,7 +5410,7 @@
       <c r="BW23" s="6"/>
       <c r="BX23" s="6"/>
       <c r="BY23" s="6"/>
-      <c r="BZ23" s="10"/>
+      <c r="BZ23" s="27"/>
       <c r="CA23" s="10"/>
       <c r="CB23" s="10"/>
       <c r="CC23" s="10"/>
@@ -5394,7 +5423,7 @@
       <c r="CJ23" s="10"/>
       <c r="CK23" s="10"/>
     </row>
-    <row r="24" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>10</v>
       </c>
@@ -5496,7 +5525,7 @@
       <c r="BW24" s="6"/>
       <c r="BX24" s="6"/>
       <c r="BY24" s="6"/>
-      <c r="BZ24" s="10"/>
+      <c r="BZ24" s="27"/>
       <c r="CA24" s="10"/>
       <c r="CB24" s="10"/>
       <c r="CC24" s="10"/>
@@ -5509,7 +5538,7 @@
       <c r="CJ24" s="10"/>
       <c r="CK24" s="10"/>
     </row>
-    <row r="25" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>10</v>
       </c>
@@ -5543,8 +5572,8 @@
       <c r="K25" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="L25" s="8">
-        <v>6</v>
+      <c r="L25" s="25" t="s">
+        <v>167</v>
       </c>
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
@@ -5611,7 +5640,7 @@
       <c r="BW25" s="6"/>
       <c r="BX25" s="6"/>
       <c r="BY25" s="6"/>
-      <c r="BZ25" s="10"/>
+      <c r="BZ25" s="27"/>
       <c r="CA25" s="10"/>
       <c r="CB25" s="10"/>
       <c r="CC25" s="10"/>
@@ -5624,7 +5653,7 @@
       <c r="CJ25" s="10"/>
       <c r="CK25" s="10"/>
     </row>
-    <row r="26" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>10</v>
       </c>
@@ -5658,8 +5687,8 @@
       <c r="K26" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="L26" s="8">
-        <v>7</v>
+      <c r="L26" s="25" t="s">
+        <v>168</v>
       </c>
       <c r="M26" s="15"/>
       <c r="N26" s="15"/>
@@ -5726,7 +5755,7 @@
       <c r="BW26" s="6"/>
       <c r="BX26" s="6"/>
       <c r="BY26" s="6"/>
-      <c r="BZ26" s="10"/>
+      <c r="BZ26" s="27"/>
       <c r="CA26" s="10"/>
       <c r="CB26" s="10"/>
       <c r="CC26" s="10"/>
@@ -5739,7 +5768,7 @@
       <c r="CJ26" s="10"/>
       <c r="CK26" s="10"/>
     </row>
-    <row r="27" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>10</v>
       </c>
@@ -5773,8 +5802,8 @@
       <c r="K27" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="8">
-        <v>8</v>
+      <c r="L27" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="M27" s="15"/>
       <c r="N27" s="15"/>
@@ -5841,7 +5870,7 @@
       <c r="BW27" s="6"/>
       <c r="BX27" s="6"/>
       <c r="BY27" s="6"/>
-      <c r="BZ27" s="10"/>
+      <c r="BZ27" s="27"/>
       <c r="CA27" s="10"/>
       <c r="CB27" s="10"/>
       <c r="CC27" s="10"/>
@@ -5854,7 +5883,7 @@
       <c r="CJ27" s="10"/>
       <c r="CK27" s="10"/>
     </row>
-    <row r="28" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>10</v>
       </c>
@@ -5888,8 +5917,8 @@
       <c r="K28" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="L28" s="8">
-        <v>9</v>
+      <c r="L28" s="25" t="s">
+        <v>169</v>
       </c>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
@@ -5956,7 +5985,7 @@
       <c r="BW28" s="6"/>
       <c r="BX28" s="6"/>
       <c r="BY28" s="6"/>
-      <c r="BZ28" s="10"/>
+      <c r="BZ28" s="27"/>
       <c r="CA28" s="10"/>
       <c r="CB28" s="10"/>
       <c r="CC28" s="10"/>
@@ -5969,7 +5998,7 @@
       <c r="CJ28" s="10"/>
       <c r="CK28" s="10"/>
     </row>
-    <row r="29" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>10</v>
       </c>
@@ -6071,7 +6100,7 @@
       <c r="BW29" s="6"/>
       <c r="BX29" s="6"/>
       <c r="BY29" s="6"/>
-      <c r="BZ29" s="10"/>
+      <c r="BZ29" s="27"/>
       <c r="CA29" s="10"/>
       <c r="CB29" s="10"/>
       <c r="CC29" s="10"/>
@@ -6084,7 +6113,7 @@
       <c r="CJ29" s="10"/>
       <c r="CK29" s="10"/>
     </row>
-    <row r="30" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>10</v>
       </c>
@@ -6186,7 +6215,7 @@
       <c r="BW30" s="6"/>
       <c r="BX30" s="6"/>
       <c r="BY30" s="6"/>
-      <c r="BZ30" s="10"/>
+      <c r="BZ30" s="27"/>
       <c r="CA30" s="10"/>
       <c r="CB30" s="10"/>
       <c r="CC30" s="10"/>
@@ -6199,7 +6228,7 @@
       <c r="CJ30" s="10"/>
       <c r="CK30" s="10"/>
     </row>
-    <row r="31" spans="1:179" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:179" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>10</v>
       </c>
@@ -6301,7 +6330,7 @@
       <c r="BW31" s="6"/>
       <c r="BX31" s="6"/>
       <c r="BY31" s="6"/>
-      <c r="BZ31" s="10"/>
+      <c r="BZ31" s="27"/>
       <c r="CA31" s="10"/>
       <c r="CB31" s="10"/>
       <c r="CC31" s="10"/>

</xml_diff>